<commit_message>
plotter v1 + reframe code
</commit_message>
<xml_diff>
--- a/database/nodes.xlsx
+++ b/database/nodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pieca\Desktop\AE4441-Group-2-VRP-Project\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C123C334-8383-4765-9766-CB92920399CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C14AD3B-3CC9-4609-933C-2BE27ABF3897}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0CE367B1-B351-42C5-9808-58DF092659A7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="10">
   <si>
     <t>lat</t>
   </si>
@@ -52,19 +52,37 @@
   </si>
   <si>
     <t>base</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>B4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -87,8 +105,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,13 +425,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30D050E7-65DF-41BC-AFB1-D09DFEC3DF85}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -426,82 +451,70 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>6.9</v>
-      </c>
-      <c r="C2">
-        <v>79</v>
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1">
+        <v>6.6846300000000003</v>
+      </c>
+      <c r="C2" s="1">
+        <v>80.734308999999996</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <f>A2+1</f>
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <f>B2+0.05</f>
-        <v>6.95</v>
-      </c>
-      <c r="C3">
-        <f>C2-0.05</f>
-        <v>78.95</v>
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1">
+        <v>7.474812</v>
+      </c>
+      <c r="C3" s="1">
+        <v>81.117546000000004</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <f t="shared" ref="A4:A15" si="0">A3+1</f>
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <f t="shared" ref="B4:B17" si="1">B3+0.05</f>
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <f t="shared" ref="C4:C17" si="2">C3-0.05</f>
-        <v>78.900000000000006</v>
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1">
+        <v>7.4980719999999996</v>
+      </c>
+      <c r="C4" s="1">
+        <v>80.361705000000001</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <f t="shared" si="1"/>
-        <v>7.05</v>
-      </c>
-      <c r="C5">
-        <f t="shared" si="2"/>
-        <v>78.850000000000009</v>
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1">
+        <v>8.7003880000000002</v>
+      </c>
+      <c r="C5" s="1">
+        <v>80.481059000000002</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <f t="shared" si="1"/>
-        <v>7.1</v>
-      </c>
-      <c r="C6">
-        <f t="shared" si="2"/>
-        <v>78.800000000000011</v>
+        <v>1</v>
+      </c>
+      <c r="B6" s="1">
+        <v>6.1888030000000001</v>
+      </c>
+      <c r="C6" s="1">
+        <v>80.519159000000002</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>
@@ -509,16 +522,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <f t="shared" si="1"/>
-        <v>7.1499999999999995</v>
-      </c>
-      <c r="C7">
-        <f t="shared" si="2"/>
-        <v>78.750000000000014</v>
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>6.2994180000000002</v>
+      </c>
+      <c r="C7" s="1">
+        <v>81.054685000000006</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
@@ -526,16 +536,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <f t="shared" si="1"/>
-        <v>7.1999999999999993</v>
-      </c>
-      <c r="C8">
-        <f t="shared" si="2"/>
-        <v>78.700000000000017</v>
+        <v>3</v>
+      </c>
+      <c r="B8" s="1">
+        <v>6.4965020000000004</v>
+      </c>
+      <c r="C8" s="1">
+        <v>80.776137000000006</v>
       </c>
       <c r="D8" t="s">
         <v>4</v>
@@ -543,16 +550,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <f t="shared" si="1"/>
-        <v>7.2499999999999991</v>
-      </c>
-      <c r="C9">
-        <f t="shared" si="2"/>
-        <v>78.65000000000002</v>
+        <v>4</v>
+      </c>
+      <c r="B9" s="1">
+        <v>6.755147</v>
+      </c>
+      <c r="C9" s="1">
+        <v>80.971558000000002</v>
       </c>
       <c r="D9" t="s">
         <v>4</v>
@@ -560,16 +564,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <f t="shared" si="1"/>
-        <v>7.2999999999999989</v>
-      </c>
-      <c r="C10">
-        <f t="shared" si="2"/>
-        <v>78.600000000000023</v>
+        <v>5</v>
+      </c>
+      <c r="B10" s="1">
+        <v>6.9784189999999997</v>
+      </c>
+      <c r="C10" s="1">
+        <v>81.246234999999999</v>
       </c>
       <c r="D10" t="s">
         <v>4</v>
@@ -577,16 +578,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <f t="shared" si="1"/>
-        <v>7.3499999999999988</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="2"/>
-        <v>78.550000000000026</v>
+        <v>6</v>
+      </c>
+      <c r="B11" s="1">
+        <v>7.4206070000000004</v>
+      </c>
+      <c r="C11" s="1">
+        <v>81.590762999999995</v>
       </c>
       <c r="D11" t="s">
         <v>4</v>
@@ -594,16 +592,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <f t="shared" si="1"/>
-        <v>7.3999999999999986</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="2"/>
-        <v>78.500000000000028</v>
+        <v>7</v>
+      </c>
+      <c r="B12" s="1">
+        <v>7.0184439999999997</v>
+      </c>
+      <c r="C12" s="1">
+        <v>80.760429000000002</v>
       </c>
       <c r="D12" t="s">
         <v>4</v>
@@ -611,16 +606,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <f t="shared" si="1"/>
-        <v>7.4499999999999984</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="2"/>
-        <v>78.450000000000031</v>
+        <v>8</v>
+      </c>
+      <c r="B13" s="1">
+        <v>7.0615059999999996</v>
+      </c>
+      <c r="C13" s="1">
+        <v>80.500652000000002</v>
       </c>
       <c r="D13" t="s">
         <v>4</v>
@@ -628,16 +620,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <f t="shared" si="1"/>
-        <v>7.4999999999999982</v>
-      </c>
-      <c r="C14">
-        <f t="shared" si="2"/>
-        <v>78.400000000000034</v>
+        <v>9</v>
+      </c>
+      <c r="B14" s="1">
+        <v>7.2213190000000003</v>
+      </c>
+      <c r="C14" s="1">
+        <v>80.055323000000001</v>
       </c>
       <c r="D14" t="s">
         <v>4</v>
@@ -645,16 +634,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <f t="shared" si="1"/>
-        <v>7.549999999999998</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="2"/>
-        <v>78.350000000000037</v>
+        <v>10</v>
+      </c>
+      <c r="B15" s="1">
+        <v>7.3261029999999998</v>
+      </c>
+      <c r="C15" s="2">
+        <v>79.904257000000001</v>
       </c>
       <c r="D15" t="s">
         <v>4</v>
@@ -662,34 +648,128 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <f t="shared" si="1"/>
-        <v>7.5999999999999979</v>
+        <v>11</v>
+      </c>
+      <c r="B16" s="1">
+        <v>7.499714</v>
       </c>
       <c r="C16">
-        <f t="shared" si="2"/>
-        <v>78.30000000000004</v>
+        <v>80.624790000000004</v>
       </c>
       <c r="D16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1">
+        <v>7.5659660000000004</v>
+      </c>
+      <c r="C17" s="1">
+        <v>80.522419999999997</v>
+      </c>
+      <c r="D17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1">
+        <v>7.6981719999999996</v>
+      </c>
+      <c r="C18" s="1">
+        <v>79.838475000000003</v>
+      </c>
+      <c r="D18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>14</v>
+      </c>
+      <c r="B19" s="1">
+        <v>8.0164679999999997</v>
+      </c>
+      <c r="C19" s="1">
+        <v>80.920918999999998</v>
+      </c>
+      <c r="D19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>15</v>
+      </c>
+      <c r="B20" s="1">
+        <v>8.6553629999999995</v>
+      </c>
+      <c r="C20">
+        <v>81.085539999999995</v>
+      </c>
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
         <v>16</v>
       </c>
-      <c r="B17">
-        <f t="shared" si="1"/>
-        <v>7.6499999999999977</v>
-      </c>
-      <c r="C17">
-        <f t="shared" si="2"/>
-        <v>78.250000000000043</v>
-      </c>
-      <c r="D17" t="s">
-        <v>5</v>
+      <c r="B21" s="1">
+        <v>8.8382679999999993</v>
+      </c>
+      <c r="C21" s="1">
+        <v>80.487302999999997</v>
+      </c>
+      <c r="D21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>17</v>
+      </c>
+      <c r="B22" s="1">
+        <v>9.1833460000000002</v>
+      </c>
+      <c r="C22" s="1">
+        <v>80.741310999999996</v>
+      </c>
+      <c r="D22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>18</v>
+      </c>
+      <c r="B23" s="1">
+        <v>9.360379</v>
+      </c>
+      <c r="C23" s="1">
+        <v>80.391710000000003</v>
+      </c>
+      <c r="D23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>19</v>
+      </c>
+      <c r="B24" s="1">
+        <v>8.8843010000000007</v>
+      </c>
+      <c r="C24" s="1">
+        <v>79.986797999999993</v>
+      </c>
+      <c r="D24" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added enekos dv, refactored
</commit_message>
<xml_diff>
--- a/database/nodes.xlsx
+++ b/database/nodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pieca\Desktop\AE4441-Group-2-VRP-Project\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5241C817-E0E1-4710-9948-2E3C45AEBF00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE91476F-E964-4FC1-86A9-30EBFD2AA9B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0CE367B1-B351-42C5-9808-58DF092659A7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
   <si>
     <t>lat</t>
   </si>
@@ -425,7 +425,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -497,7 +497,7 @@
         <v>80.361705000000001</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -518,7 +518,7 @@
         <v>4</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -536,28 +536,98 @@
         <v>4</v>
       </c>
       <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>6.2994180000000002</v>
+      </c>
+      <c r="C7" s="1">
+        <v>81.054685000000006</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>6.4965020000000004</v>
+      </c>
+      <c r="C8" s="1">
+        <v>80.776137000000006</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>6.755147</v>
+      </c>
+      <c r="C9" s="1">
+        <v>80.971558000000002</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>6.9784189999999997</v>
+      </c>
+      <c r="C10" s="1">
+        <v>81.246234999999999</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-    </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>7.4206070000000004</v>
+      </c>
+      <c r="C11" s="1">
+        <v>81.590762999999995</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>

</xml_diff>

<commit_message>
fixed dv + priority
</commit_message>
<xml_diff>
--- a/database/nodes.xlsx
+++ b/database/nodes.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pieca\Desktop\AE4441-Group-2-VRP-Project\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE91476F-E964-4FC1-86A9-30EBFD2AA9B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC314CD2-250B-49B3-9BF8-D21979F17B24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0CE367B1-B351-42C5-9808-58DF092659A7}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
+    <sheet name="full_nodes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="7">
   <si>
     <t>lat</t>
   </si>
@@ -422,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30D050E7-65DF-41BC-AFB1-D09DFEC3DF85}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -433,7 +434,7 @@
     <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -450,7 +451,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -467,53 +468,54 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
-        <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="1">
+        <v>7.0184439999999997</v>
+      </c>
+      <c r="C3" s="1">
+        <v>80.760429000000002</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f>A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
         <v>7.474812</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C4" s="1">
         <v>81.117546000000004</v>
       </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <f t="shared" ref="A4:A11" si="0">A3+1</f>
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f t="shared" ref="A5:A11" si="0">A4+1</f>
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
         <v>7.4980719999999996</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C5" s="1">
         <v>80.361705000000001</v>
       </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>8.7003880000000002</v>
-      </c>
-      <c r="C5" s="1">
-        <v>80.481059000000002</v>
-      </c>
       <c r="D5" t="s">
         <v>4</v>
       </c>
@@ -521,16 +523,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>6.1888030000000001</v>
+        <v>8.7003880000000002</v>
       </c>
       <c r="C6" s="1">
-        <v>80.519159000000002</v>
+        <v>80.481059000000002</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>
@@ -538,149 +540,429 @@
       <c r="E6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>6.2994180000000002</v>
+        <v>6.1888030000000001</v>
       </c>
       <c r="C7" s="1">
-        <v>81.054685000000006</v>
+        <v>80.519159000000002</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
       </c>
       <c r="E7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>6.4965020000000004</v>
+        <v>6.2994180000000002</v>
       </c>
       <c r="C8" s="1">
-        <v>80.776137000000006</v>
+        <v>81.054685000000006</v>
       </c>
       <c r="D8" t="s">
         <v>4</v>
       </c>
       <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>6.755147</v>
+        <v>6.4965020000000004</v>
       </c>
       <c r="C9" s="1">
-        <v>80.971558000000002</v>
+        <v>80.776137000000006</v>
       </c>
       <c r="D9" t="s">
         <v>4</v>
       </c>
       <c r="E9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>6.9784189999999997</v>
+        <v>6.755147</v>
       </c>
       <c r="C10" s="1">
-        <v>81.246234999999999</v>
+        <v>80.971558000000002</v>
       </c>
       <c r="D10" t="s">
         <v>4</v>
       </c>
       <c r="E10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>7.4206070000000004</v>
+        <v>6.9784189999999997</v>
       </c>
       <c r="C11" s="1">
-        <v>81.590762999999995</v>
+        <v>81.246234999999999</v>
       </c>
       <c r="D11" t="s">
         <v>4</v>
       </c>
       <c r="E11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B15" s="1"/>
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H16" s="1"/>
+    </row>
+    <row r="18" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="20" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H20" s="1"/>
+    </row>
+    <row r="22" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="24" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B4A54AA-6135-479F-885E-D73F66E12E68}">
+  <dimension ref="A1:I24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <f>nodes!A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B2" s="1">
+        <v>7.0615059999999996</v>
+      </c>
+      <c r="C2" s="1">
+        <v>80.500652000000002</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
+        <v>7.2213190000000003</v>
+      </c>
+      <c r="C3" s="1">
+        <v>80.055323000000001</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f>A3+1</f>
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>7.3261029999999998</v>
+      </c>
+      <c r="C4" s="2">
+        <v>79.904257000000001</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f>A4+1</f>
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>7.499714</v>
+      </c>
+      <c r="C5">
+        <v>80.624790000000004</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f>A5+1</f>
+        <v>7</v>
+      </c>
+      <c r="B6" s="1">
+        <v>7.5659660000000004</v>
+      </c>
+      <c r="C6" s="1">
+        <v>80.522419999999997</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f>A6+1</f>
+        <v>8</v>
+      </c>
+      <c r="B7" s="1">
+        <v>7.6981719999999996</v>
+      </c>
+      <c r="C7" s="1">
+        <v>79.838475000000003</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f>A7+1</f>
+        <v>9</v>
+      </c>
+      <c r="B8" s="1">
+        <v>8.0164679999999997</v>
+      </c>
+      <c r="C8" s="1">
+        <v>80.920918999999998</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f>A8+1</f>
+        <v>10</v>
+      </c>
+      <c r="B9" s="1">
+        <v>8.6553629999999995</v>
+      </c>
+      <c r="C9">
+        <v>81.085539999999995</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f>A9+1</f>
+        <v>11</v>
+      </c>
+      <c r="B10" s="1">
+        <v>8.8382679999999993</v>
+      </c>
+      <c r="C10" s="1">
+        <v>80.487302999999997</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f>A10+1</f>
+        <v>12</v>
+      </c>
+      <c r="B11" s="1">
+        <v>9.1833460000000002</v>
+      </c>
+      <c r="C11" s="1">
+        <v>80.741310999999996</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f>A11+1</f>
+        <v>13</v>
+      </c>
+      <c r="B12" s="1">
+        <v>9.360379</v>
+      </c>
+      <c r="C12" s="1">
+        <v>80.391710000000003</v>
+      </c>
+      <c r="D12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f>A12+1</f>
+        <v>14</v>
+      </c>
+      <c r="B13" s="1">
+        <v>8.8843010000000007</v>
+      </c>
+      <c r="C13" s="1">
+        <v>79.986797999999993</v>
+      </c>
+      <c r="D13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="1"/>
+      <c r="C15" s="2"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
results code, bad written
</commit_message>
<xml_diff>
--- a/database/nodes.xlsx
+++ b/database/nodes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pieca\Desktop\AE4441-Group-2-VRP-Project\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27CCACA8-BD89-4245-9F74-F3BC320349BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE7EE02-84DF-4351-A5D1-85161C3A65A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0CE367B1-B351-42C5-9808-58DF092659A7}"/>
+    <workbookView xWindow="33480" yWindow="1215" windowWidth="17280" windowHeight="8970" xr2:uid="{0CE367B1-B351-42C5-9808-58DF092659A7}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
@@ -425,8 +425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30D050E7-65DF-41BC-AFB1-D09DFEC3DF85}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -508,7 +508,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f t="shared" ref="A5:A18" si="0">A4+1</f>
+        <f t="shared" ref="A5:A15" si="0">A4+1</f>
         <v>4</v>
       </c>
       <c r="B5">
@@ -561,7 +561,7 @@
         <v>4</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -617,7 +617,7 @@
         <v>4</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -637,7 +637,7 @@
         <v>4</v>
       </c>
       <c r="E11">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -712,7 +712,7 @@
         <v>4</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -730,7 +730,7 @@
         <v>4</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H16" s="1"/>
     </row>
@@ -749,7 +749,7 @@
         <v>4</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -767,7 +767,7 @@
         <v>4</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H18" s="1"/>
     </row>

</xml_diff>

<commit_message>
fixed plotter, fuck this
</commit_message>
<xml_diff>
--- a/database/nodes.xlsx
+++ b/database/nodes.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pieca\Desktop\AE4441-Group-2-VRP-Project\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5EBB85C-F3A7-4497-B90E-8DE5168B3EF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F71FF15-C8BD-4371-B841-BE0276F914E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0CE367B1-B351-42C5-9808-58DF092659A7}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
-    <sheet name="full_nodes" sheetId="2" r:id="rId2"/>
+    <sheet name="backup" sheetId="3" r:id="rId2"/>
+    <sheet name="full_nodes" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="7">
   <si>
     <t>lat</t>
   </si>
@@ -425,8 +426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30D050E7-65DF-41BC-AFB1-D09DFEC3DF85}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -470,6 +471,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
+        <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3">
@@ -487,39 +489,37 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f>A3+1</f>
+        <f t="shared" ref="A4:A16" si="0">A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>7.53</v>
-      </c>
-      <c r="C4">
-        <f>360-278.6431503</f>
-        <v>81.356849699999998</v>
+      <c r="B4" s="1">
+        <v>6.1888030000000001</v>
+      </c>
+      <c r="C4" s="1">
+        <v>80.519159000000002</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f t="shared" ref="A5:A15" si="0">A4+1</f>
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>7.16289394</v>
-      </c>
-      <c r="C5">
-        <f>360-279.42956539</f>
-        <v>80.570434610000007</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>6.9784189999999997</v>
+      </c>
+      <c r="C5" s="1">
+        <v>81.246234999999999</v>
       </c>
       <c r="D5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -530,15 +530,14 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>6.6514617200000004</v>
-      </c>
-      <c r="C6">
-        <f>360-279.30078505</f>
-        <v>80.699214949999998</v>
+      <c r="B6" s="1">
+        <v>7.0184439999999997</v>
+      </c>
+      <c r="C6" s="1">
+        <v>80.760429000000002</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -552,16 +551,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>6.1888030000000001</v>
+        <v>7.2213190000000003</v>
       </c>
       <c r="C7" s="1">
-        <v>80.519159000000002</v>
+        <v>80.055323000000001</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -570,16 +569,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>6.9784189999999997</v>
-      </c>
-      <c r="C8" s="1">
-        <v>81.246234999999999</v>
+        <v>7.499714</v>
+      </c>
+      <c r="C8">
+        <v>80.624790000000004</v>
       </c>
       <c r="D8" t="s">
         <v>4</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -590,10 +589,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>7.0184439999999997</v>
+        <v>8.0164679999999997</v>
       </c>
       <c r="C9" s="1">
-        <v>80.760429000000002</v>
+        <v>80.920918999999998</v>
       </c>
       <c r="D9" t="s">
         <v>4</v>
@@ -608,194 +607,57 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>7.2213190000000003</v>
+        <v>9.360379</v>
       </c>
       <c r="C10" s="1">
-        <v>80.055323000000001</v>
+        <v>80.391710000000003</v>
       </c>
       <c r="D10" t="s">
         <v>4</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B11" s="1">
-        <v>7.499714</v>
-      </c>
-      <c r="C11">
-        <v>80.624790000000004</v>
-      </c>
-      <c r="D11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B12" s="1">
-        <v>8.0164679999999997</v>
-      </c>
-      <c r="C12" s="1">
-        <v>80.920918999999998</v>
-      </c>
-      <c r="D12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B13" s="1">
-        <v>9.360379</v>
-      </c>
-      <c r="C13" s="1">
-        <v>80.391710000000003</v>
-      </c>
-      <c r="D13" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
+      <c r="B13" s="1"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B14" s="1">
-        <v>8.8843010000000007</v>
-      </c>
-      <c r="C14" s="1">
-        <v>79.986797999999993</v>
-      </c>
-      <c r="D14" t="s">
-        <v>4</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B15" s="1">
-        <v>7.4206070000000004</v>
-      </c>
-      <c r="C15" s="1">
-        <v>81.590762999999995</v>
-      </c>
-      <c r="D15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <f>A15+1</f>
-        <v>15</v>
-      </c>
-      <c r="B16" s="1">
-        <v>8.6553629999999995</v>
-      </c>
-      <c r="C16">
-        <v>81.085539999999995</v>
-      </c>
-      <c r="D16" t="s">
-        <v>4</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <f>A16+1</f>
-        <v>16</v>
-      </c>
-      <c r="B17" s="1">
-        <v>8.8382679999999993</v>
-      </c>
-      <c r="C17" s="1">
-        <v>80.487302999999997</v>
-      </c>
-      <c r="D17" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <f>A17+1</f>
-        <v>17</v>
-      </c>
-      <c r="B18" s="1">
-        <v>8.7003880000000002</v>
-      </c>
-      <c r="C18" s="1">
-        <v>80.481059000000002</v>
-      </c>
-      <c r="D18" t="s">
-        <v>4</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
+    <row r="18" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <f>A18+1</f>
-        <v>18</v>
-      </c>
-      <c r="B19" s="1">
-        <v>8.8843010000000007</v>
-      </c>
-      <c r="C19" s="1">
-        <v>79.986797999999993</v>
-      </c>
-      <c r="D19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H20" s="1"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H22" s="1"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H24" s="1"/>
     </row>
   </sheetData>
@@ -805,6 +667,363 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82EDB126-A5ED-4373-AC0F-EA18BF9358B3}">
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>8.3305389999999999</v>
+      </c>
+      <c r="C2">
+        <v>80.411660999999995</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>9.0450049999999997</v>
+      </c>
+      <c r="C3">
+        <v>80.518867999999998</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f>A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>7.53</v>
+      </c>
+      <c r="C4">
+        <f>360-278.6431503</f>
+        <v>81.356849699999998</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f t="shared" ref="A5:A15" si="0">A4+1</f>
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>7.16289394</v>
+      </c>
+      <c r="C5">
+        <f>360-279.42956539</f>
+        <v>80.570434610000007</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>6.6514617200000004</v>
+      </c>
+      <c r="C6">
+        <f>360-279.30078505</f>
+        <v>80.699214949999998</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>6.1888030000000001</v>
+      </c>
+      <c r="C7" s="1">
+        <v>80.519159000000002</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>6.9784189999999997</v>
+      </c>
+      <c r="C8" s="1">
+        <v>81.246234999999999</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>7.0184439999999997</v>
+      </c>
+      <c r="C9" s="1">
+        <v>80.760429000000002</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>7.2213190000000003</v>
+      </c>
+      <c r="C10" s="1">
+        <v>80.055323000000001</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>7.499714</v>
+      </c>
+      <c r="C11">
+        <v>80.624790000000004</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>8.0164679999999997</v>
+      </c>
+      <c r="C12" s="1">
+        <v>80.920918999999998</v>
+      </c>
+      <c r="D12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>9.360379</v>
+      </c>
+      <c r="C13" s="1">
+        <v>80.391710000000003</v>
+      </c>
+      <c r="D13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>8.8843010000000007</v>
+      </c>
+      <c r="C14" s="1">
+        <v>79.986797999999993</v>
+      </c>
+      <c r="D14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>7.4206070000000004</v>
+      </c>
+      <c r="C15" s="1">
+        <v>81.590762999999995</v>
+      </c>
+      <c r="D15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <f>A15+1</f>
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>8.6553629999999995</v>
+      </c>
+      <c r="C16">
+        <v>81.085539999999995</v>
+      </c>
+      <c r="D16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f>A16+1</f>
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>8.8382679999999993</v>
+      </c>
+      <c r="C17" s="1">
+        <v>80.487302999999997</v>
+      </c>
+      <c r="D17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <f>A17+1</f>
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>8.7003880000000002</v>
+      </c>
+      <c r="C18" s="1">
+        <v>80.481059000000002</v>
+      </c>
+      <c r="D18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <f>A18+1</f>
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>8.8843010000000007</v>
+      </c>
+      <c r="C19" s="1">
+        <v>79.986797999999993</v>
+      </c>
+      <c r="D19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B4A54AA-6135-479F-885E-D73F66E12E68}">
   <dimension ref="A1:I24"/>
   <sheetViews>

</xml_diff>